<commit_message>
update total  commit number
</commit_message>
<xml_diff>
--- a/BadSmell/results/group_vs_issuenum/group_vs_issuenum.xlsx
+++ b/BadSmell/results/group_vs_issuenum/group_vs_issuenum.xlsx
@@ -221,46 +221,46 @@
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>group11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>group10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>group13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>group12</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>group14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>group5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>group4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>group7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>group6</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>group1</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="10">
+                  <c:v>group3</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>group2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>group3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>group4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>group5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>group6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>group7</c:v>
-                </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
+                  <c:v>group9</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>group8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>group9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>group10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>group11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>group12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>group13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>group14</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -272,46 +272,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>38.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.0</c:v>
+                  <c:v>81.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62.0</c:v>
+                  <c:v>53.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>98.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>57.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>86.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>87.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>90.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>52.0</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>85.0</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>32.0</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>56.0</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>53.0</c:v>
+                  <c:v>51.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>96.0</c:v>
+                  <c:v>89.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -328,11 +328,11 @@
         </c:dLbls>
         <c:gapWidth val="63"/>
         <c:overlap val="-24"/>
-        <c:axId val="-2081768272"/>
-        <c:axId val="-2101306192"/>
+        <c:axId val="-2042817264"/>
+        <c:axId val="-2042672272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2081768272"/>
+        <c:axId val="-2042817264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -371,7 +371,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101306192"/>
+        <c:crossAx val="-2042672272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -379,7 +379,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2101306192"/>
+        <c:axId val="-2042672272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -388,7 +388,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2081768272"/>
+        <c:crossAx val="-2042817264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1248,7 +1248,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1263,114 +1263,114 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>98</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>57</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>87</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>52</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>85</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>56</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update commit history trend non-linearity score
</commit_message>
<xml_diff>
--- a/BadSmell/results/group_vs_issuenum/group_vs_issuenum.xlsx
+++ b/BadSmell/results/group_vs_issuenum/group_vs_issuenum.xlsx
@@ -221,46 +221,46 @@
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>group1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>group2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>group3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>group4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>group5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>group6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>group7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>group8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>group9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>group10</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>group11</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>group10</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>group12</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>group13</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>group12</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="13">
                   <c:v>group14</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>group5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>group4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>group7</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>group6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>group1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>group3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>group2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>group9</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>group8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -272,46 +272,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>98.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>81.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>31.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>81.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>53.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="13">
                   <c:v>96.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>56.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>98.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>86.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>58.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>89.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -328,11 +328,11 @@
         </c:dLbls>
         <c:gapWidth val="63"/>
         <c:overlap val="-24"/>
-        <c:axId val="-2042817264"/>
-        <c:axId val="-2042672272"/>
+        <c:axId val="-2019504848"/>
+        <c:axId val="-2019501728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2042817264"/>
+        <c:axId val="-2019504848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -371,7 +371,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2042672272"/>
+        <c:crossAx val="-2019501728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -379,7 +379,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2042672272"/>
+        <c:axId val="-2019501728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -388,7 +388,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2042817264"/>
+        <c:crossAx val="-2019504848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1248,7 +1248,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1263,114 +1263,114 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>53</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>56</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>96</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>80</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B10">
-        <v>86</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>37</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>32</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>89</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>